<commit_message>
Add IsPrint arg to error_handling.py; add demo.ipynb
</commit_message>
<xml_diff>
--- a/libs/ErrorCodes.xlsx
+++ b/libs/ErrorCodes.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Box Sync\Projects\Python_ErrorHandling\libs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092A9B24-553E-4E3D-B4C2-B0AD8AFCB390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C08B31-E6FB-4D3B-A922-6EF46344FFC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="1785" windowWidth="28800" windowHeight="11587" xr2:uid="{CD3C727C-9923-402D-B728-1749A83ECA6F}"/>
+    <workbookView xWindow="98" yWindow="0" windowWidth="30217" windowHeight="18473" xr2:uid="{CD3C727C-9923-402D-B728-1749A83ECA6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Errors_" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,41 +35,12 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>j.d.landgrebe</author>
-  </authors>
-  <commentList>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{1B56E87D-3662-4DBD-B8FA-DCA7D205BD93}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>False = developer-facing error such as VBA Error; True = user-facing warning or error message</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="40">
   <si>
     <t>iCode</t>
   </si>
   <si>
-    <t>sVal</t>
-  </si>
-  <si>
-    <t>iMsgDevUser</t>
-  </si>
-  <si>
     <t>Base</t>
   </si>
   <si>
@@ -95,6 +66,96 @@
   </si>
   <si>
     <t>Error but no base row for Locn</t>
+  </si>
+  <si>
+    <t>ProceduralDemo</t>
+  </si>
+  <si>
+    <t>ERROR: x + y should be less than or equal to 4. Sum</t>
+  </si>
+  <si>
+    <t>SumAndProduct</t>
+  </si>
+  <si>
+    <t>calculate_sum</t>
+  </si>
+  <si>
+    <t>calculate_product</t>
+  </si>
+  <si>
+    <t>ERROR: x + y should be less than or equal to 6. Sum</t>
+  </si>
+  <si>
+    <t>ERROR: x * y should be less than or equal to 5. Product</t>
+  </si>
+  <si>
+    <t>CheckExcelFiles</t>
+  </si>
+  <si>
+    <t>CheckFilesProcedure</t>
+  </si>
+  <si>
+    <t>ERROR: Input file not found</t>
+  </si>
+  <si>
+    <t>ERROR: Input file not a valid Excel file</t>
+  </si>
+  <si>
+    <t>ERROR: Required input file sheet not found</t>
+  </si>
+  <si>
+    <t>CheckDataFrame</t>
+  </si>
+  <si>
+    <t>ColNonBlank</t>
+  </si>
+  <si>
+    <t>ERROR: Required column is blank</t>
+  </si>
+  <si>
+    <t>ContainsRequiredCols</t>
+  </si>
+  <si>
+    <t>ERROR: Required column not present</t>
+  </si>
+  <si>
+    <t>ColAllNumeric</t>
+  </si>
+  <si>
+    <t>ColAllPopulated</t>
+  </si>
+  <si>
+    <t>ERROR: All column values must be non-blank</t>
+  </si>
+  <si>
+    <t>IndexContainsListVals</t>
+  </si>
+  <si>
+    <t>ERROR: Index must contain all specified values</t>
+  </si>
+  <si>
+    <t>ColumnsContainListVals</t>
+  </si>
+  <si>
+    <t>ERROR: DataFrame Columns must contain all specified values</t>
+  </si>
+  <si>
+    <t>ERROR: DataFrame Column cannot be blank</t>
+  </si>
+  <si>
+    <t>NoDuplicateColVals</t>
+  </si>
+  <si>
+    <t>ERROR: DataFrame Column values must be unique</t>
+  </si>
+  <si>
+    <t>NoDuplicateCols</t>
+  </si>
+  <si>
+    <t>ERROR: DataFrame cannot have duplicate columns and names cannot end in ".x" where x is a digit</t>
+  </si>
+  <si>
+    <t>ERROR: Column must contain only non-blank numeric values for the col_b column</t>
   </si>
 </sst>
 </file>
@@ -123,13 +184,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,6 +209,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -157,12 +243,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -171,8 +258,17 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{E6D5D499-F2AF-460A-868B-D7ADACE0D124}"/>
@@ -486,93 +582,468 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{616FF38B-CF99-49A7-8EA0-C0A3E18AA1A1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{616FF38B-CF99-49A7-8EA0-C0A3E18AA1A1}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="5.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="58.9296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.73046875" customWidth="1"/>
-    <col min="6" max="6" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="7">
+        <v>10</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="7">
+        <v>11</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="9">
+        <v>20</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="2">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" s="2">
         <v>100</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="2">
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="2">
         <v>101</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>105</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="2">
+        <v>102</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="2">
+        <v>103</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="6">
+        <v>110</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" s="6">
+        <v>111</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" s="6">
+        <v>115</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" s="6">
+        <v>116</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" s="6">
+        <v>120</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" s="6">
+        <v>121</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" s="6">
+        <v>125</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16" s="6">
+        <v>126</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" s="6">
+        <v>130</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" s="6">
+        <v>131</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" s="6">
+        <v>135</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" s="6">
+        <v>136</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" s="6">
+        <v>140</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" s="6">
+        <v>147</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" s="6">
+        <v>140</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" s="6">
+        <v>148</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" s="6">
+        <v>140</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" s="6">
+        <v>141</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" s="4">
+        <v>200</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D27" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" s="4">
+        <v>201</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" s="5">
+        <v>300</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" s="5">
+        <v>301</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" s="5">
+        <v>310</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" s="5">
+        <v>311</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update to recent changes in local error codes; switch to testing preflight with ErrorCodes.xlsx
</commit_message>
<xml_diff>
--- a/libs/ErrorCodes.xlsx
+++ b/libs/ErrorCodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Box Sync\Projects\Python_ErrorHandling\libs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C08B31-E6FB-4D3B-A922-6EF46344FFC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CBD38E-85D9-4422-9E85-ADBEB222F386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="98" yWindow="0" windowWidth="30217" windowHeight="18473" xr2:uid="{CD3C727C-9923-402D-B728-1749A83ECA6F}"/>
+    <workbookView xWindow="907" yWindow="1208" windowWidth="28403" windowHeight="17415" xr2:uid="{CD3C727C-9923-402D-B728-1749A83ECA6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Errors_" sheetId="1" r:id="rId1"/>
@@ -155,7 +155,7 @@
     <t>ERROR: DataFrame cannot have duplicate columns and names cannot end in ".x" where x is a digit</t>
   </si>
   <si>
-    <t>ERROR: Column must contain only non-blank numeric values for the col_b column</t>
+    <t>ERROR: Column must contain only non-blank numeric values</t>
   </si>
 </sst>
 </file>
@@ -249,7 +249,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -266,6 +266,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
@@ -287,9 +288,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -327,7 +328,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -433,7 +434,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -575,7 +576,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -587,7 +588,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -726,7 +727,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="6">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>22</v>
@@ -740,7 +741,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="6">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>22</v>
@@ -754,7 +755,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="6">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>22</v>
@@ -767,8 +768,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13" s="6">
-        <v>120</v>
+      <c r="A13" s="10">
+        <v>150</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>22</v>
@@ -781,8 +782,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" s="6">
-        <v>121</v>
+      <c r="A14" s="10">
+        <v>155</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>22</v>
@@ -795,8 +796,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15" s="6">
-        <v>125</v>
+      <c r="A15" s="10">
+        <v>170</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>22</v>
@@ -809,8 +810,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" s="6">
-        <v>126</v>
+      <c r="A16" s="10">
+        <v>174</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>22</v>
@@ -823,8 +824,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" s="6">
-        <v>130</v>
+      <c r="A17" s="10">
+        <v>190</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>22</v>
@@ -837,8 +838,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" s="6">
-        <v>131</v>
+      <c r="A18" s="10">
+        <v>193</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>22</v>
@@ -851,8 +852,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" s="6">
-        <v>135</v>
+      <c r="A19" s="10">
+        <v>210</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>22</v>
@@ -865,8 +866,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" s="6">
-        <v>136</v>
+      <c r="A20" s="10">
+        <v>212</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>22</v>
@@ -879,8 +880,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" s="6">
-        <v>140</v>
+      <c r="A21" s="10">
+        <v>230</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>22</v>
@@ -893,8 +894,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" s="6">
-        <v>147</v>
+      <c r="A22" s="10">
+        <v>237</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>22</v>
@@ -907,8 +908,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A23" s="6">
-        <v>140</v>
+      <c r="A23" s="10">
+        <v>250</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>22</v>
@@ -921,8 +922,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A24" s="6">
-        <v>148</v>
+      <c r="A24" s="10">
+        <v>258</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>22</v>
@@ -935,8 +936,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A25" s="6">
-        <v>140</v>
+      <c r="A25" s="10">
+        <v>270</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>22</v>
@@ -949,8 +950,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26" s="6">
-        <v>141</v>
+      <c r="A26" s="10">
+        <v>271</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>22</v>
@@ -964,7 +965,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
@@ -976,7 +977,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
-        <v>201</v>
+        <v>401</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4" t="s">
@@ -988,7 +989,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="5">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>12</v>
@@ -1002,7 +1003,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="5">
-        <v>301</v>
+        <v>501</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>12</v>
@@ -1016,7 +1017,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="5">
-        <v>310</v>
+        <v>510</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>12</v>
@@ -1030,7 +1031,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="5">
-        <v>311</v>
+        <v>511</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Changes through 2/26/24 from work on client project
</commit_message>
<xml_diff>
--- a/libs/ErrorCodes.xlsx
+++ b/libs/ErrorCodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Box Sync\Projects\Python_ErrorHandling\libs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3795E29-AA57-48A1-8E33-F064FEB224D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FEF1B4-760F-48E4-8C6C-F3EA2C1ADC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="907" yWindow="1208" windowWidth="28403" windowHeight="17415" xr2:uid="{CD3C727C-9923-402D-B728-1749A83ECA6F}"/>
+    <workbookView xWindow="1410" yWindow="1410" windowWidth="28800" windowHeight="11332" xr2:uid="{CD3C727C-9923-402D-B728-1749A83ECA6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Errors_" sheetId="1" r:id="rId1"/>
@@ -587,7 +587,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -727,7 +727,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="6">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Refactoring; add tests for all preflight.py methods
</commit_message>
<xml_diff>
--- a/libs/ErrorCodes.xlsx
+++ b/libs/ErrorCodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Box Sync\Projects\Python_ErrorHandling\libs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F301E022-F334-4312-8700-82B5B18C6DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A0D418-5832-4E0E-B223-EDABF25E9BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33157" yWindow="1395" windowWidth="22732" windowHeight="13628" xr2:uid="{CD3C727C-9923-402D-B728-1749A83ECA6F}"/>
+    <workbookView xWindow="1103" yWindow="1103" windowWidth="22732" windowHeight="13627" xr2:uid="{CD3C727C-9923-402D-B728-1749A83ECA6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Errors_" sheetId="1" r:id="rId1"/>
@@ -678,8 +678,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -804,7 +804,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="6">
-        <v>130</v>
+        <v>200</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>22</v>
@@ -818,7 +818,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="10">
-        <v>131</v>
+        <v>201</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>22</v>
@@ -832,7 +832,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="10">
-        <v>150</v>
+        <v>220</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>22</v>
@@ -846,7 +846,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="10">
-        <v>152</v>
+        <v>222</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>22</v>
@@ -860,7 +860,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="10">
-        <v>170</v>
+        <v>240</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>22</v>
@@ -874,7 +874,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="10">
-        <v>173</v>
+        <v>243</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>22</v>
@@ -888,7 +888,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="10">
-        <v>190</v>
+        <v>260</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>22</v>
@@ -902,7 +902,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="10">
-        <v>194</v>
+        <v>264</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>22</v>
@@ -916,7 +916,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="10">
-        <v>210</v>
+        <v>280</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>22</v>
@@ -930,7 +930,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="10">
-        <v>215</v>
+        <v>285</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>22</v>
@@ -944,7 +944,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="10">
-        <v>230</v>
+        <v>300</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>22</v>
@@ -958,7 +958,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="10">
-        <v>236</v>
+        <v>306</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>22</v>
@@ -972,7 +972,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="6">
-        <v>250</v>
+        <v>320</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>22</v>
@@ -986,7 +986,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="10">
-        <v>257</v>
+        <v>327</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>22</v>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="10">
-        <v>270</v>
+        <v>340</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>22</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="10">
-        <v>278</v>
+        <v>348</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>22</v>
@@ -1028,7 +1028,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="10">
-        <v>290</v>
+        <v>360</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>22</v>
@@ -1042,7 +1042,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="10">
-        <v>299</v>
+        <v>369</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>22</v>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="10">
-        <v>310</v>
+        <v>380</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>22</v>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="10">
-        <v>320</v>
+        <v>390</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>22</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="10">
-        <v>330</v>
+        <v>400</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>22</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="10">
-        <v>341</v>
+        <v>411</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>22</v>
@@ -1112,7 +1112,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="10">
-        <v>350</v>
+        <v>420</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>22</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="10">
-        <v>362</v>
+        <v>432</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>22</v>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="10">
-        <v>370</v>
+        <v>440</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>22</v>
@@ -1154,7 +1154,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="10">
-        <v>383</v>
+        <v>453</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>22</v>
@@ -1168,7 +1168,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="10">
-        <v>390</v>
+        <v>460</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>22</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="10">
-        <v>404</v>
+        <v>474</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
delete tbls testing from this repo. demo.ipynb update for ErrorHandle and preflights
</commit_message>
<xml_diff>
--- a/libs/ErrorCodes.xlsx
+++ b/libs/ErrorCodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Box Sync\Projects\Python_ErrorHandling\libs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A0D418-5832-4E0E-B223-EDABF25E9BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAA9EFC-DFB3-4E09-9B12-C919B0256650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1103" yWindow="1103" windowWidth="22732" windowHeight="13627" xr2:uid="{CD3C727C-9923-402D-B728-1749A83ECA6F}"/>
+    <workbookView xWindow="-37335" yWindow="1433" windowWidth="32812" windowHeight="11857" xr2:uid="{CD3C727C-9923-402D-B728-1749A83ECA6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Errors_" sheetId="1" r:id="rId1"/>
@@ -678,8 +678,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:E36"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" s="4">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="B65" s="4"/>
       <c r="C65" s="4" t="s">
@@ -1600,7 +1600,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" s="4">
-        <v>501</v>
+        <v>1001</v>
       </c>
       <c r="B66" s="4"/>
       <c r="C66" s="4" t="s">
@@ -1612,7 +1612,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" s="5">
-        <v>600</v>
+        <v>1100</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>12</v>
@@ -1626,7 +1626,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" s="5">
-        <v>601</v>
+        <v>1101</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>12</v>
@@ -1640,7 +1640,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" s="5">
-        <v>610</v>
+        <v>1102</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>12</v>
@@ -1654,7 +1654,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" s="5">
-        <v>611</v>
+        <v>1103</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>12</v>

</xml_diff>